<commit_message>
cleaned up test print output
cleaned up test print output
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -19,13 +19,13 @@
     <t>Name:</t>
   </si>
   <si>
-    <t>justin</t>
+    <t>justin ossai</t>
   </si>
   <si>
     <t>CSU ID:</t>
   </si>
   <si>
-    <t>12345678</t>
+    <t>123456789</t>
   </si>
   <si>
     <t>Path to Graduation</t>

</xml_diff>

<commit_message>
condensed code for year input fix
condensed code for year input fix
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
   <si>
     <t>Name:</t>
   </si>
@@ -25,7 +25,7 @@
     <t>CSU ID:</t>
   </si>
   <si>
-    <t>123</t>
+    <t>1234</t>
   </si>
   <si>
     <t>Path to Graduation</t>
@@ -40,25 +40,16 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Fall 2023</t>
+    <t>Fall 2024</t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Spring 2023</t>
-  </si>
-  <si>
-    <t>ITDS 1779 - Scholarship Across the Disciplines []</t>
-  </si>
-  <si>
-    <t>CPSC 1302K - Computer Science II (minimum grade of C) []</t>
-  </si>
-  <si>
-    <t>CPSC 2105 - Computer Organization (minimum grade of C) ['Fa', 'Sp']</t>
-  </si>
-  <si>
-    <t>Fall 2024</t>
+    <t>Spring 2024</t>
+  </si>
+  <si>
+    <t>Fall 2025</t>
   </si>
   <si>
     <t>CPSC 2108 - Data Structures (minimum grade of C) ['Fa', 'Sp']</t>
@@ -70,7 +61,7 @@
     <t>ASTR 1105 &amp; ASTR 1305 - Descriptive Astronomy: The Solar Systemand Descriptive Astronomy Lab (lab optional) []</t>
   </si>
   <si>
-    <t>Spring 2024</t>
+    <t>Spring 2025</t>
   </si>
   <si>
     <t>STAT 1401 - Elementary Statistics []</t>
@@ -79,7 +70,7 @@
     <t>CPSC 3175 - Object-Oriented Design (minimum grade of C) ['Fa', 'Sp']</t>
   </si>
   <si>
-    <t>Fall 2025</t>
+    <t>Fall 2026</t>
   </si>
   <si>
     <t>CPSC 3125 - Operating Systems (minimum grade of C) ['Fa', 'Sp']</t>
@@ -91,7 +82,7 @@
     <t>CPSC 3XXX - CPSC 3000 level or above []</t>
   </si>
   <si>
-    <t>Spring 2025</t>
+    <t>Spring 2026</t>
   </si>
   <si>
     <t>CPSC 3165 - Professionalism in Computing (minimum grade of C) ['Fa', 'Sp']</t>
@@ -100,7 +91,7 @@
     <t>CPSC 4175 - Software Engineering (minimum grade of C) ['Fa', '--']</t>
   </si>
   <si>
-    <t>Fall 2026</t>
+    <t>Fall 2027</t>
   </si>
   <si>
     <t>CPSC 4155 - Computer Architecture (minimum grade of C) []</t>
@@ -109,7 +100,7 @@
     <t>CPSC 4157 - Computer Networks (minimum grade of C) []</t>
   </si>
   <si>
-    <t>Spring 2026</t>
+    <t>Spring 2027</t>
   </si>
   <si>
     <t>CPSC 4000 - Baccalaureate Survey ['Fa', 'Sp']</t>
@@ -689,49 +680,31 @@
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-    </row>
     <row r="6" spans="1:8">
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -739,7 +712,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="F7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -747,15 +720,15 @@
     </row>
     <row r="8" spans="1:8">
       <c r="F8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="F9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G9">
         <v>3</v>
@@ -763,7 +736,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="F10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -785,27 +758,30 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G11">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -813,19 +789,19 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G13">
         <v>3</v>
@@ -833,77 +809,58 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D14">
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G14">
-        <v>2</v>
-      </c>
-      <c r="H14" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G15">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="F16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:7">
       <c r="F17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="F18" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="F19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:7">
       <c r="A20" s="4" t="s">
         <v>9</v>
       </c>
@@ -918,64 +875,58 @@
         <f>SUM(D13:D19)</f>
         <v>0</v>
       </c>
-      <c r="F20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B24">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:7">
       <c r="A29" s="4" t="s">
         <v>9</v>
       </c>
@@ -991,43 +942,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:7">
       <c r="A30" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
         <v>29</v>
-      </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31" t="s">
-        <v>32</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
         <v>30</v>
-      </c>
-      <c r="B32">
-        <v>3</v>
-      </c>
-      <c r="C32" t="s">
-        <v>33</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -1035,7 +986,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="C33" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -1059,10 +1010,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="C39" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D39" s="6">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>